<commit_message>
rédaction du readme final pour la présentation du projet
</commit_message>
<xml_diff>
--- a/data/actifs.xlsx
+++ b/data/actifs.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guilhembarroyer/Desktop/Projects/Finance_verte/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F48BBA7-7BC3-5347-9FD3-850FC04300B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A93732A-AB4C-E84A-B6CF-EE17932B3561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{45D35138-28E4-4213-B1AD-03D64D52A638}"/>
+    <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="17500" xr2:uid="{45D35138-28E4-4213-B1AD-03D64D52A638}"/>
   </bookViews>
   <sheets>
     <sheet name="Entreprises" sheetId="1" r:id="rId1"/>
-    <sheet name="Fonds" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Entreprises!$A$1:$L$47</definedName>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
   <si>
     <t>Actions</t>
   </si>
@@ -87,9 +86,6 @@
     <t>ALO.PA</t>
   </si>
   <si>
-    <t>Finansol</t>
-  </si>
-  <si>
     <t>Arkema</t>
   </si>
   <si>
@@ -333,280 +329,10 @@
     <t>SPIE.PA</t>
   </si>
   <si>
-    <t>Fonds labélisés ISR</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> SGP (Société de Gestion de Portefeuille)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> FONDS </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CLASSE D'ACTIFS </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> FOCUS GÉO </t>
-  </si>
-  <si>
-    <t>ISIN</t>
-  </si>
-  <si>
-    <t>AMPERE GESTION</t>
-  </si>
-  <si>
-    <t>FONDS DE LOGEMENT INTERMÉDIAIRE II - FLI II</t>
-  </si>
-  <si>
-    <t>Immobilier</t>
-  </si>
-  <si>
-    <t>France</t>
-  </si>
-  <si>
-    <t>FR0013384047</t>
-  </si>
-  <si>
-    <t>EIFFEL INVESTMENT GROUP</t>
-  </si>
-  <si>
-    <t>HARMONIE MUTUELLE EMPLOIS France</t>
-  </si>
-  <si>
-    <t>Diversifié</t>
-  </si>
-  <si>
-    <t>FR0007496039</t>
-  </si>
-  <si>
-    <t>LA FRANÇAISE REM</t>
-  </si>
-  <si>
-    <t>SCPI LA FRANÇAISE GRAND PARIS PATRIMOINE</t>
-  </si>
-  <si>
-    <t>IIUFG000LGPP</t>
-  </si>
-  <si>
-    <t>LBO France Gestion</t>
-  </si>
-  <si>
-    <t>France Développement</t>
-  </si>
-  <si>
-    <t>FR0014001012</t>
-  </si>
-  <si>
-    <t>France Engagement</t>
-  </si>
-  <si>
-    <t>LU1885494549</t>
-  </si>
-  <si>
-    <t>MANDARINE GESTION</t>
-  </si>
-  <si>
-    <t>Mandarine Opportunités</t>
-  </si>
-  <si>
-    <t>FR0010657122</t>
-  </si>
-  <si>
-    <t>NORMA CAPITAL</t>
-  </si>
-  <si>
-    <t>SCPI FAIR INVEST</t>
-  </si>
-  <si>
-    <t>SCPI00004429</t>
-  </si>
-  <si>
-    <t>SYCOMORE ASSET MANAGEMENT</t>
-  </si>
-  <si>
-    <t>SYCOMORE SÉLECTION CRÉDIT</t>
-  </si>
-  <si>
-    <t>Obligations</t>
-  </si>
-  <si>
-    <t>Europe</t>
-  </si>
-  <si>
-    <t>FR0011288513</t>
-  </si>
-  <si>
-    <t>SG 29 HAUSSMANN</t>
-  </si>
-  <si>
-    <t>SG Echiquier Actions France Diversifié ISR</t>
-  </si>
-  <si>
-    <t>FR0013535549</t>
-  </si>
-  <si>
-    <t>Mirova (Natixis)</t>
-  </si>
-  <si>
-    <t>Mirova Women Leaders Equity Fund</t>
-  </si>
-  <si>
-    <t>Monde</t>
-  </si>
-  <si>
-    <t>FR0013187176</t>
-  </si>
-  <si>
-    <t>Amundi</t>
-  </si>
-  <si>
-    <t>Amundi Ethik und Solidarität</t>
-  </si>
-  <si>
-    <t>Mixte</t>
-  </si>
-  <si>
-    <t>AT0000A1EL54</t>
-  </si>
-  <si>
-    <t>FNG-Siegel</t>
-  </si>
-  <si>
-    <t>BNP Paribas AM</t>
-  </si>
-  <si>
-    <t>BNP Paribas Social Business France</t>
-  </si>
-  <si>
-    <t>FR0013170750</t>
-  </si>
-  <si>
-    <t>La Banque Postale AM</t>
-  </si>
-  <si>
-    <t>LBPAM ISR Actions Solidaire</t>
-  </si>
-  <si>
-    <t>FR0010708768</t>
-  </si>
-  <si>
-    <t>Sycomore AM</t>
-  </si>
-  <si>
-    <t>Sycomore Happy@Work</t>
-  </si>
-  <si>
-    <t>FR0010971721</t>
-  </si>
-  <si>
-    <t>Towards Sustainability</t>
-  </si>
-  <si>
-    <t>OFI Asset Management</t>
-  </si>
-  <si>
-    <t>OFI RS Engagement for a Fair Society</t>
-  </si>
-  <si>
-    <t>FR0013267150</t>
-  </si>
-  <si>
-    <t>CPR Asset Management</t>
-  </si>
-  <si>
-    <t>CPR Social Impact</t>
-  </si>
-  <si>
-    <t>FR0013053154</t>
-  </si>
-  <si>
-    <t>Ecofi Investissements</t>
-  </si>
-  <si>
-    <t>Ecofi Agir pour le Climat</t>
-  </si>
-  <si>
-    <t>FR0010642280</t>
-  </si>
-  <si>
-    <t>HSBC Global AM</t>
-  </si>
-  <si>
-    <t>HSBC SRI Global Equity</t>
-  </si>
-  <si>
-    <t>FR0000438905</t>
-  </si>
-  <si>
-    <t>Fonds de VC/PE spécialisés dans l'impact social</t>
-  </si>
-  <si>
-    <t>Citizen Capital </t>
-  </si>
-  <si>
-    <t>Alter Equity</t>
-  </si>
-  <si>
-    <t>Mirova</t>
-  </si>
-  <si>
-    <t>La Nef</t>
-  </si>
-  <si>
-    <t>Time for the Planet</t>
-  </si>
-  <si>
-    <t>SWEN Capital Partners</t>
-  </si>
-  <si>
-    <t>Esfin Gestion</t>
-  </si>
-  <si>
-    <t>Inco Ventures</t>
-  </si>
-  <si>
-    <t>Mandalore Impact debt fund</t>
-  </si>
-  <si>
-    <t>Phitrust</t>
-  </si>
-  <si>
-    <t>Obligations sociales</t>
-  </si>
-  <si>
-    <t>Amundi Impact Social Bund</t>
-  </si>
-  <si>
-    <t>Obligations Sociales de la République Française (OAT Sociales)</t>
-  </si>
-  <si>
-    <t>Obligations Sociales de la Ville de Paris</t>
-  </si>
-  <si>
-    <t>Obligations Sociales de la Ville de Marseille</t>
-  </si>
-  <si>
-    <t>Obligations Sociales de la Région Île-de-France </t>
-  </si>
-  <si>
-    <t>Obligations Sociales de la Caisse d'Amortissement de la Dette Sociale (CADES)</t>
-  </si>
-  <si>
-    <t>Obligations Sociales de la Banque Européenne d'Investissement (BEI)</t>
-  </si>
-  <si>
     <t>Boite française</t>
   </si>
   <si>
     <t>Score Social YahooFinance normalisé</t>
-  </si>
-  <si>
-    <t>Greenfin</t>
-  </si>
-  <si>
-    <t>Article 9 SDFR</t>
-  </si>
-  <si>
-    <t>Autres</t>
   </si>
   <si>
     <t>SPIE</t>
@@ -631,10 +357,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-  </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -657,38 +380,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -708,7 +401,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -721,21 +414,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -768,31 +446,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -822,19 +476,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -858,13 +499,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -873,51 +513,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="17" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="17" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="17" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1261,13 +872,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="67.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.5" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37.1640625" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="29" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="34.5" style="4" customWidth="1"/>
+    <col min="9" max="9" width="34.5" style="3" customWidth="1"/>
     <col min="10" max="10" width="8.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="32.5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
@@ -1277,50 +888,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="32" t="s">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="G1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="H1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="32" t="s">
-        <v>185</v>
-      </c>
-      <c r="J1" s="33" t="s">
-        <v>194</v>
-      </c>
-      <c r="K1" s="32" t="s">
+      <c r="I1" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="K1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="34" t="s">
-        <v>184</v>
-      </c>
-      <c r="M1" s="6"/>
+      <c r="L1" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="M1" s="5"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>20</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>21</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1340,28 +951,28 @@
       <c r="H2">
         <v>10.3</v>
       </c>
-      <c r="I2" s="35">
-        <f ca="1">(H2-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
+      <c r="I2" s="17">
+        <f t="shared" ref="I2:I47" ca="1" si="0">(H2-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
         <v>0.58227848101265833</v>
       </c>
-      <c r="J2" s="36">
+      <c r="J2" s="18">
         <f ca="1">1.2*C2 + 1.2*D2 + 0.5*E2 + F2 + G2 - I2 - 0.15*K2</f>
         <v>3.8677215189873415</v>
       </c>
       <c r="K2">
         <v>3</v>
       </c>
-      <c r="L2" s="22">
-        <v>1</v>
-      </c>
-      <c r="M2" s="35"/>
+      <c r="L2" s="10">
+        <v>1</v>
+      </c>
+      <c r="M2" s="17"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>22</v>
-      </c>
-      <c r="B3" s="22" t="s">
-        <v>23</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1381,28 +992,28 @@
       <c r="H3">
         <v>13.6</v>
       </c>
-      <c r="I3" s="35">
-        <f ca="1">(H3-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
+      <c r="I3" s="17">
+        <f t="shared" ca="1" si="0"/>
         <v>0.79113924050632922</v>
       </c>
-      <c r="J3" s="36">
+      <c r="J3" s="18">
         <f ca="1">1.2*C3 + 1.2*D3 + 0.5*E3 + F3 + G3 - I3 - 0.15*K3</f>
         <v>2.3088607594936708</v>
       </c>
       <c r="K3">
         <v>2</v>
       </c>
-      <c r="L3" s="22">
+      <c r="L3" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="B4" s="22" t="s">
-        <v>89</v>
-      </c>
       <c r="C4">
         <v>1</v>
       </c>
@@ -1412,37 +1023,37 @@
       <c r="E4">
         <v>0</v>
       </c>
-      <c r="F4" s="4">
-        <v>0</v>
-      </c>
-      <c r="G4" s="5">
-        <v>0</v>
-      </c>
-      <c r="H4" s="5">
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0</v>
+      </c>
+      <c r="H4" s="4">
         <v>6.3</v>
       </c>
-      <c r="I4" s="35">
-        <f ca="1">(H4-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
+      <c r="I4" s="17">
+        <f t="shared" ca="1" si="0"/>
         <v>0.32911392405063289</v>
       </c>
-      <c r="J4" s="36">
+      <c r="J4" s="18">
         <f ca="1">1.2*C4 + 1.2*D4 + 0.5*E4 + F4 + G4 - I4 - 0.1*K4</f>
         <v>1.8708860759493671</v>
       </c>
       <c r="K4">
         <v>2</v>
       </c>
-      <c r="L4" s="22">
+      <c r="L4" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="B5" s="22" t="s">
-        <v>94</v>
-      </c>
       <c r="C5">
         <v>0</v>
       </c>
@@ -1452,36 +1063,36 @@
       <c r="E5">
         <v>0</v>
       </c>
-      <c r="F5" s="4">
-        <v>0</v>
-      </c>
-      <c r="G5" s="5">
-        <v>1</v>
-      </c>
-      <c r="H5" s="5">
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="4">
+        <v>1</v>
+      </c>
+      <c r="H5" s="4">
         <v>3.2</v>
       </c>
-      <c r="I5" s="35">
-        <f ca="1">(H5-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
+      <c r="I5" s="17">
+        <f t="shared" ca="1" si="0"/>
         <v>0.13291139240506331</v>
       </c>
-      <c r="J5" s="36">
+      <c r="J5" s="18">
         <f ca="1">1.2*C5 + 1.2*D5 + 0.5*E5 + F5 + G5 - I5 - 0.15*K5</f>
         <v>1.767088607594937</v>
       </c>
       <c r="K5">
         <v>2</v>
       </c>
-      <c r="L5" s="22">
+      <c r="L5" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>96</v>
+        <v>98</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>95</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -1501,27 +1112,27 @@
       <c r="H6">
         <v>6.1</v>
       </c>
-      <c r="I6" s="35">
-        <f ca="1">(H6-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
+      <c r="I6" s="17">
+        <f t="shared" ca="1" si="0"/>
         <v>0.31645569620253167</v>
       </c>
-      <c r="J6" s="36">
+      <c r="J6" s="18">
         <f ca="1">1.2*C6 + 1.2*D6 + 0.5*E6 + F6 + G6 - I6 - 0.15*K6</f>
         <v>1.7335443037974687</v>
       </c>
       <c r="K6">
         <v>1</v>
       </c>
-      <c r="L6" s="22">
+      <c r="L6" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>75</v>
-      </c>
-      <c r="B7" s="22" t="s">
-        <v>76</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1541,27 +1152,27 @@
       <c r="H7">
         <v>9.1</v>
       </c>
-      <c r="I7" s="35">
-        <f ca="1">(H7-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
+      <c r="I7" s="17">
+        <f t="shared" ca="1" si="0"/>
         <v>0.50632911392405067</v>
       </c>
-      <c r="J7" s="36">
+      <c r="J7" s="18">
         <f ca="1">1.2*C7 + 1.2*D7 + 0.5*E7 + F7 + G7 - I7 - 0.15*K7</f>
         <v>1.6936708860759493</v>
       </c>
       <c r="K7">
         <v>2</v>
       </c>
-      <c r="L7" s="22">
+      <c r="L7" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>87</v>
+        <v>102</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>86</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1572,36 +1183,36 @@
       <c r="E8">
         <v>0</v>
       </c>
-      <c r="F8" s="4">
-        <v>0</v>
-      </c>
-      <c r="G8" s="5">
-        <v>0</v>
-      </c>
-      <c r="H8" s="5">
+      <c r="F8" s="3">
+        <v>0</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0</v>
+      </c>
+      <c r="H8" s="4">
         <v>7.8</v>
       </c>
-      <c r="I8" s="35">
-        <f ca="1">(H8-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
+      <c r="I8" s="17">
+        <f t="shared" ca="1" si="0"/>
         <v>0.42405063291139239</v>
       </c>
-      <c r="J8" s="36">
+      <c r="J8" s="18">
         <f ca="1">1.2*C8 + 1.2*D8 + 0.5*E8 + F8 + G8 - I8 - 0.1*K8</f>
         <v>1.7759493670886075</v>
       </c>
       <c r="K8">
         <v>2</v>
       </c>
-      <c r="L8" s="22">
+      <c r="L8" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>71</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>72</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1621,28 +1232,28 @@
       <c r="H9">
         <v>8.8000000000000007</v>
       </c>
-      <c r="I9" s="35">
-        <f ca="1">(H9-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
+      <c r="I9" s="17">
+        <f t="shared" ca="1" si="0"/>
         <v>0.48734177215189883</v>
       </c>
-      <c r="J9" s="36">
+      <c r="J9" s="18">
         <f ca="1">1.2*C9 + 1.2*D9 + 0.5*E9 + F9 + G9 - I9 - 0.15*K9</f>
         <v>1.5626582278481014</v>
       </c>
       <c r="K9">
         <v>3</v>
       </c>
-      <c r="L9" s="22">
+      <c r="L9" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="B10" s="22" t="s">
-        <v>82</v>
-      </c>
       <c r="C10">
         <v>1</v>
       </c>
@@ -1652,36 +1263,36 @@
       <c r="E10">
         <v>0</v>
       </c>
-      <c r="F10" s="4">
-        <v>0</v>
-      </c>
-      <c r="G10" s="5">
-        <v>1</v>
-      </c>
-      <c r="H10" s="5">
+      <c r="F10" s="3">
+        <v>0</v>
+      </c>
+      <c r="G10" s="4">
+        <v>1</v>
+      </c>
+      <c r="H10" s="4">
         <v>5.9</v>
       </c>
-      <c r="I10" s="35">
-        <f ca="1">(H10-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
+      <c r="I10" s="17">
+        <f t="shared" ca="1" si="0"/>
         <v>0.30379746835443044</v>
       </c>
-      <c r="J10" s="36">
+      <c r="J10" s="18">
         <f ca="1">1.2*C10 + 1.2*D10 + 0.5*E10 + F10 + G10 - I10 - 0.1*K10</f>
         <v>1.6962025316455698</v>
       </c>
       <c r="K10">
         <v>2</v>
       </c>
-      <c r="L10" s="22">
+      <c r="L10" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>34</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>35</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -1701,18 +1312,18 @@
       <c r="H11">
         <v>6.9</v>
       </c>
-      <c r="I11" s="35">
-        <f ca="1">(H11-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
+      <c r="I11" s="17">
+        <f t="shared" ca="1" si="0"/>
         <v>0.36708860759493678</v>
       </c>
-      <c r="J11" s="36">
+      <c r="J11" s="18">
         <f ca="1">1.2*C11 + 1.2*D11 + 0.5*E11 + F11 + G11 - I11 - 0.15*K11</f>
         <v>1.4829113924050632</v>
       </c>
       <c r="K11">
         <v>1</v>
       </c>
-      <c r="L11" s="22">
+      <c r="L11" s="10">
         <v>1</v>
       </c>
     </row>
@@ -1720,7 +1331,7 @@
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C12">
@@ -1741,27 +1352,27 @@
       <c r="H12">
         <v>5.8</v>
       </c>
-      <c r="I12" s="35">
-        <f ca="1">(H12-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
+      <c r="I12" s="17">
+        <f t="shared" ca="1" si="0"/>
         <v>0.29746835443037972</v>
       </c>
-      <c r="J12" s="36">
+      <c r="J12" s="18">
         <f ca="1">1.2*C12 + 1.2*D12 + 0.5*E12 + F12 + G12 - I12 - 0.15*K12</f>
         <v>1.4025316455696202</v>
       </c>
       <c r="K12">
         <v>2</v>
       </c>
-      <c r="L12" s="22">
+      <c r="L12" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>79</v>
-      </c>
-      <c r="B13" s="22" t="s">
-        <v>80</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1781,27 +1392,27 @@
       <c r="H13">
         <v>11.5</v>
       </c>
-      <c r="I13" s="35">
-        <f ca="1">(H13-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
+      <c r="I13" s="17">
+        <f t="shared" ca="1" si="0"/>
         <v>0.65822784810126589</v>
       </c>
-      <c r="J13" s="36">
+      <c r="J13" s="18">
         <f ca="1">1.2*C13 + 1.2*D13 + 0.5*E13 + F13 + G13 - I13 - 0.15*K13</f>
         <v>1.3917721518987343</v>
       </c>
       <c r="K13">
         <v>3</v>
       </c>
-      <c r="L13" s="22">
+      <c r="L13" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="10" t="s">
         <v>18</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>19</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1821,28 +1432,28 @@
       <c r="H14">
         <v>9.3000000000000007</v>
       </c>
-      <c r="I14" s="35">
-        <f ca="1">(H14-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
+      <c r="I14" s="17">
+        <f t="shared" ca="1" si="0"/>
         <v>0.518987341772152</v>
       </c>
-      <c r="J14" s="36">
+      <c r="J14" s="18">
         <f ca="1">1.2*C14 + 1.2*D14 + 0.5*E14 + F14 + G14 - I14 - 0.15*K14</f>
         <v>1.181012658227848</v>
       </c>
       <c r="K14">
         <v>2</v>
       </c>
-      <c r="L14" s="22">
+      <c r="L14" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="B15" s="22" t="s">
-        <v>86</v>
-      </c>
       <c r="C15">
         <v>0</v>
       </c>
@@ -1852,36 +1463,36 @@
       <c r="E15">
         <v>0</v>
       </c>
-      <c r="F15" s="4">
-        <v>1</v>
-      </c>
-      <c r="G15" s="5">
-        <v>1</v>
-      </c>
-      <c r="H15" s="5">
+      <c r="F15" s="3">
+        <v>1</v>
+      </c>
+      <c r="G15" s="4">
+        <v>1</v>
+      </c>
+      <c r="H15" s="4">
         <v>10.199999999999999</v>
       </c>
-      <c r="I15" s="35">
-        <f ca="1">(H15-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
+      <c r="I15" s="17">
+        <f t="shared" ca="1" si="0"/>
         <v>0.57594936708860767</v>
       </c>
-      <c r="J15" s="36">
+      <c r="J15" s="18">
         <f ca="1">1.2*C15 + 1.2*D15 + 0.5*E15 + F15 + G15 - I15 - 0.1*K15</f>
         <v>1.2240506329113925</v>
       </c>
       <c r="K15">
         <v>2</v>
       </c>
-      <c r="L15" s="22">
+      <c r="L15" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>26</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>27</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1901,27 +1512,27 @@
       <c r="H16">
         <v>10.3</v>
       </c>
-      <c r="I16" s="35">
-        <f ca="1">(H16-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
+      <c r="I16" s="17">
+        <f t="shared" ca="1" si="0"/>
         <v>0.58227848101265833</v>
       </c>
-      <c r="J16" s="36">
-        <f t="shared" ref="J16:J27" ca="1" si="0">1.2*C16 + 1.2*D16 + 0.5*E16 + F16 + G16 - I16 - 0.15*K16</f>
+      <c r="J16" s="18">
+        <f t="shared" ref="J16:J27" ca="1" si="1">1.2*C16 + 1.2*D16 + 0.5*E16 + F16 + G16 - I16 - 0.15*K16</f>
         <v>1.1177215189873417</v>
       </c>
       <c r="K16">
         <v>2</v>
       </c>
-      <c r="L16" s="22">
+      <c r="L16" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="10" t="s">
         <v>43</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>44</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1941,27 +1552,27 @@
       <c r="H17">
         <v>3.5</v>
       </c>
-      <c r="I17" s="35">
-        <f ca="1">(H17-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
+      <c r="I17" s="17">
+        <f t="shared" ca="1" si="0"/>
         <v>0.15189873417721519</v>
       </c>
-      <c r="J17" s="36">
-        <f t="shared" ca="1" si="0"/>
+      <c r="J17" s="18">
+        <f t="shared" ca="1" si="1"/>
         <v>1.0481012658227848</v>
       </c>
       <c r="K17">
         <v>2</v>
       </c>
-      <c r="L17" s="22">
+      <c r="L17" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="10" t="s">
         <v>61</v>
-      </c>
-      <c r="B18" s="22" t="s">
-        <v>62</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1981,27 +1592,27 @@
       <c r="H18">
         <v>4</v>
       </c>
-      <c r="I18" s="35">
-        <f ca="1">(H18-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
+      <c r="I18" s="17">
+        <f t="shared" ca="1" si="0"/>
         <v>0.18354430379746836</v>
       </c>
-      <c r="J18" s="36">
-        <f t="shared" ca="1" si="0"/>
+      <c r="J18" s="18">
+        <f t="shared" ca="1" si="1"/>
         <v>1.0164556962025315</v>
       </c>
       <c r="K18">
         <v>2</v>
       </c>
-      <c r="L18" s="22">
+      <c r="L18" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="10" t="s">
         <v>24</v>
-      </c>
-      <c r="B19" s="22" t="s">
-        <v>25</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -2021,27 +1632,27 @@
       <c r="H19">
         <v>4.5</v>
       </c>
-      <c r="I19" s="35">
-        <f ca="1">(H19-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
+      <c r="I19" s="17">
+        <f t="shared" ca="1" si="0"/>
         <v>0.21518987341772153</v>
       </c>
-      <c r="J19" s="36">
-        <f t="shared" ca="1" si="0"/>
+      <c r="J19" s="18">
+        <f t="shared" ca="1" si="1"/>
         <v>0.9848101265822784</v>
       </c>
       <c r="K19">
         <v>2</v>
       </c>
-      <c r="L19" s="22">
+      <c r="L19" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="10" t="s">
         <v>65</v>
-      </c>
-      <c r="B20" s="22" t="s">
-        <v>66</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -2061,27 +1672,27 @@
       <c r="H20">
         <v>11.2</v>
       </c>
-      <c r="I20" s="35">
-        <f ca="1">(H20-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
+      <c r="I20" s="17">
+        <f t="shared" ca="1" si="0"/>
         <v>0.639240506329114</v>
       </c>
-      <c r="J20" s="36">
-        <f t="shared" ca="1" si="0"/>
+      <c r="J20" s="18">
+        <f t="shared" ca="1" si="1"/>
         <v>0.91075949367088604</v>
       </c>
       <c r="K20">
         <v>3</v>
       </c>
-      <c r="L20" s="22">
+      <c r="L20" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="B21" s="22" t="s">
-        <v>92</v>
+        <v>101</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>91</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -2092,36 +1703,36 @@
       <c r="E21">
         <v>0</v>
       </c>
-      <c r="F21" s="4">
-        <v>0</v>
-      </c>
-      <c r="G21" s="5">
-        <v>0</v>
-      </c>
-      <c r="H21" s="5">
+      <c r="F21" s="3">
+        <v>0</v>
+      </c>
+      <c r="G21" s="4">
+        <v>0</v>
+      </c>
+      <c r="H21" s="4">
         <v>4.8</v>
       </c>
-      <c r="I21" s="35">
-        <f ca="1">(H21-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
+      <c r="I21" s="17">
+        <f t="shared" ca="1" si="0"/>
         <v>0.23417721518987342</v>
       </c>
-      <c r="J21" s="36">
-        <f t="shared" ca="1" si="0"/>
+      <c r="J21" s="18">
+        <f t="shared" ca="1" si="1"/>
         <v>0.81582278481012649</v>
       </c>
       <c r="K21">
         <v>1</v>
       </c>
-      <c r="L21" s="22">
+      <c r="L21" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="10" t="s">
         <v>39</v>
-      </c>
-      <c r="B22" s="22" t="s">
-        <v>40</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -2141,27 +1752,27 @@
       <c r="H22">
         <v>7.4</v>
       </c>
-      <c r="I22" s="35">
-        <f ca="1">(H22-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
+      <c r="I22" s="17">
+        <f t="shared" ca="1" si="0"/>
         <v>0.39873417721518994</v>
       </c>
-      <c r="J22" s="36">
-        <f t="shared" ca="1" si="0"/>
+      <c r="J22" s="18">
+        <f t="shared" ca="1" si="1"/>
         <v>0.80126582278480996</v>
       </c>
       <c r="K22">
         <v>2</v>
       </c>
-      <c r="L22" s="22">
+      <c r="L22" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="10" t="s">
         <v>57</v>
-      </c>
-      <c r="B23" s="22" t="s">
-        <v>58</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -2181,27 +1792,27 @@
       <c r="H23">
         <v>6.7</v>
       </c>
-      <c r="I23" s="35">
-        <f ca="1">(H23-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
+      <c r="I23" s="17">
+        <f t="shared" ca="1" si="0"/>
         <v>0.35443037974683544</v>
       </c>
-      <c r="J23" s="36">
-        <f t="shared" ca="1" si="0"/>
+      <c r="J23" s="18">
+        <f t="shared" ca="1" si="1"/>
         <v>0.69556962025316449</v>
       </c>
       <c r="K23">
         <v>3</v>
       </c>
-      <c r="L23" s="22">
+      <c r="L23" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="10" t="s">
         <v>55</v>
-      </c>
-      <c r="B24" s="22" t="s">
-        <v>56</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -2221,27 +1832,27 @@
       <c r="H24">
         <v>12.7</v>
       </c>
-      <c r="I24" s="35">
-        <f ca="1">(H24-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
+      <c r="I24" s="17">
+        <f t="shared" ca="1" si="0"/>
         <v>0.73417721518987344</v>
       </c>
-      <c r="J24" s="36">
-        <f t="shared" ca="1" si="0"/>
+      <c r="J24" s="18">
+        <f t="shared" ca="1" si="1"/>
         <v>0.61582278481012653</v>
       </c>
       <c r="K24">
         <v>1</v>
       </c>
-      <c r="L24" s="22">
+      <c r="L24" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="10" t="s">
         <v>53</v>
-      </c>
-      <c r="B25" s="22" t="s">
-        <v>54</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -2261,27 +1872,27 @@
       <c r="H25">
         <v>5.2</v>
       </c>
-      <c r="I25" s="35">
-        <f ca="1">(H25-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
+      <c r="I25" s="17">
+        <f t="shared" ca="1" si="0"/>
         <v>0.25949367088607594</v>
       </c>
-      <c r="J25" s="36">
-        <f t="shared" ca="1" si="0"/>
+      <c r="J25" s="18">
+        <f t="shared" ca="1" si="1"/>
         <v>0.59050632911392398</v>
       </c>
       <c r="K25">
         <v>1</v>
       </c>
-      <c r="L25" s="22">
+      <c r="L25" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="10" t="s">
         <v>51</v>
-      </c>
-      <c r="B26" s="22" t="s">
-        <v>52</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -2301,27 +1912,27 @@
       <c r="H26">
         <v>8.6999999999999993</v>
       </c>
-      <c r="I26" s="35">
-        <f ca="1">(H26-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
+      <c r="I26" s="17">
+        <f t="shared" ca="1" si="0"/>
         <v>0.48101265822784811</v>
       </c>
-      <c r="J26" s="36">
-        <f t="shared" ca="1" si="0"/>
+      <c r="J26" s="18">
+        <f t="shared" ca="1" si="1"/>
         <v>0.56898734177215204</v>
       </c>
       <c r="K26">
         <v>3</v>
       </c>
-      <c r="L26" s="22">
+      <c r="L26" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" s="10" t="s">
         <v>63</v>
-      </c>
-      <c r="B27" s="22" t="s">
-        <v>64</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -2341,28 +1952,28 @@
       <c r="H27">
         <v>10</v>
       </c>
-      <c r="I27" s="35">
-        <f ca="1">(H27-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
+      <c r="I27" s="17">
+        <f t="shared" ca="1" si="0"/>
         <v>0.56329113924050644</v>
       </c>
-      <c r="J27" s="36">
-        <f t="shared" ca="1" si="0"/>
+      <c r="J27" s="18">
+        <f t="shared" ca="1" si="1"/>
         <v>0.4867088607594936</v>
       </c>
       <c r="K27">
         <v>3</v>
       </c>
-      <c r="L27" s="22">
+      <c r="L27" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B28" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="B28" s="22" t="s">
-        <v>91</v>
-      </c>
       <c r="C28">
         <v>0</v>
       </c>
@@ -2372,36 +1983,36 @@
       <c r="E28">
         <v>0</v>
       </c>
-      <c r="F28" s="4">
-        <v>0</v>
-      </c>
-      <c r="G28" s="5">
-        <v>1</v>
-      </c>
-      <c r="H28" s="5">
+      <c r="F28" s="3">
+        <v>0</v>
+      </c>
+      <c r="G28" s="4">
+        <v>1</v>
+      </c>
+      <c r="H28" s="4">
         <v>6.4</v>
       </c>
-      <c r="I28" s="35">
-        <f ca="1">(H28-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
+      <c r="I28" s="17">
+        <f t="shared" ca="1" si="0"/>
         <v>0.33544303797468361</v>
       </c>
-      <c r="J28" s="36">
+      <c r="J28" s="18">
         <f ca="1">1.2*C28 + 1.2*D28 + 0.5*E28 + F28 + G28 - I28 - 0.1*K28</f>
         <v>0.56455696202531647</v>
       </c>
       <c r="K28">
         <v>1</v>
       </c>
-      <c r="L28" s="22">
+      <c r="L28" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B29" s="10" t="s">
         <v>77</v>
-      </c>
-      <c r="B29" s="22" t="s">
-        <v>78</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -2421,27 +2032,27 @@
       <c r="H29">
         <v>7</v>
       </c>
-      <c r="I29" s="35">
-        <f ca="1">(H29-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
+      <c r="I29" s="17">
+        <f t="shared" ca="1" si="0"/>
         <v>0.37341772151898739</v>
       </c>
-      <c r="J29" s="36">
+      <c r="J29" s="18">
         <f ca="1">1.2*C29 + 1.2*D29 + 0.5*E29 + F29 + G29 - I29 - 0.15*K29</f>
         <v>0.47658227848101264</v>
       </c>
       <c r="K29">
         <v>1</v>
       </c>
-      <c r="L29" s="22">
+      <c r="L29" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="10" t="s">
         <v>59</v>
-      </c>
-      <c r="B30" s="22" t="s">
-        <v>60</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -2461,27 +2072,27 @@
       <c r="H30">
         <v>11.9</v>
       </c>
-      <c r="I30" s="35">
-        <f ca="1">(H30-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
+      <c r="I30" s="17">
+        <f t="shared" ca="1" si="0"/>
         <v>0.68354430379746844</v>
       </c>
-      <c r="J30" s="36">
+      <c r="J30" s="18">
         <f ca="1">1.2*C30 + 1.2*D30 + 0.5*E30 + F30 + G30 - I30 - 0.15*K30</f>
         <v>0.3664556962025316</v>
       </c>
       <c r="K30">
         <v>3</v>
       </c>
-      <c r="L30" s="22">
+      <c r="L30" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" s="10" t="s">
         <v>73</v>
-      </c>
-      <c r="B31" s="22" t="s">
-        <v>74</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -2501,27 +2112,27 @@
       <c r="H31">
         <v>1.1000000000000001</v>
       </c>
-      <c r="I31" s="35">
-        <f ca="1">(H31-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
-        <v>0</v>
-      </c>
-      <c r="J31" s="36">
+      <c r="I31" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J31" s="18">
         <f ca="1">1.2*C31 + 1.2*D31 + 0.5*E31 + F31 + G31 - I31 - 0.15*K31</f>
         <v>0.35</v>
       </c>
       <c r="K31">
         <v>1</v>
       </c>
-      <c r="L31" s="22">
+      <c r="L31" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="10" t="s">
         <v>32</v>
-      </c>
-      <c r="B32" s="22" t="s">
-        <v>33</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -2541,18 +2152,18 @@
       <c r="H32">
         <v>7</v>
       </c>
-      <c r="I32" s="35">
-        <f ca="1">(H32-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
+      <c r="I32" s="17">
+        <f t="shared" ca="1" si="0"/>
         <v>0.37341772151898739</v>
       </c>
-      <c r="J32" s="36">
+      <c r="J32" s="18">
         <f ca="1">1.2*C32 + 1.2*D32 + 0.5*E32 + F32 + G32 - I32 - 0.15*K32</f>
         <v>0.32658227848101268</v>
       </c>
       <c r="K32">
         <v>2</v>
       </c>
-      <c r="L32" s="22">
+      <c r="L32" s="10">
         <v>1</v>
       </c>
     </row>
@@ -2560,7 +2171,7 @@
       <c r="A33" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B33" s="22" t="s">
+      <c r="B33" s="10" t="s">
         <v>12</v>
       </c>
       <c r="C33">
@@ -2581,28 +2192,28 @@
       <c r="H33">
         <v>12.6</v>
       </c>
-      <c r="I33" s="35">
-        <f ca="1">(H33-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
+      <c r="I33" s="17">
+        <f t="shared" ca="1" si="0"/>
         <v>0.72784810126582289</v>
       </c>
-      <c r="J33" s="36">
+      <c r="J33" s="18">
         <f ca="1">1.2*C33 + 1.2*D33 + 0.5*E33 + F33 + G33 - I33 - 0.15*K33</f>
         <v>0.32215189873417716</v>
       </c>
       <c r="K33">
         <v>3</v>
       </c>
-      <c r="L33" s="22">
+      <c r="L33" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B34" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B34" s="22" t="s">
-        <v>84</v>
-      </c>
       <c r="C34">
         <v>0</v>
       </c>
@@ -2612,36 +2223,36 @@
       <c r="E34">
         <v>0</v>
       </c>
-      <c r="F34" s="4">
-        <v>0</v>
-      </c>
-      <c r="G34" s="5">
-        <v>0</v>
-      </c>
-      <c r="H34" s="5">
+      <c r="F34" s="3">
+        <v>0</v>
+      </c>
+      <c r="G34" s="4">
+        <v>0</v>
+      </c>
+      <c r="H34" s="4">
         <v>11.4</v>
       </c>
-      <c r="I34" s="35">
-        <f ca="1">(H34-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
+      <c r="I34" s="17">
+        <f t="shared" ca="1" si="0"/>
         <v>0.65189873417721533</v>
       </c>
-      <c r="J34" s="36">
+      <c r="J34" s="18">
         <f ca="1">1.2*C34 + 1.2*D34 + 0.5*E34 + F34 + G34 - I34 - 0.1*K34</f>
         <v>0.34810126582278461</v>
       </c>
       <c r="K34">
         <v>2</v>
       </c>
-      <c r="L34" s="22">
+      <c r="L34" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="B35" s="22" t="s">
-        <v>95</v>
+        <v>99</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>94</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -2652,36 +2263,36 @@
       <c r="E35">
         <v>0</v>
       </c>
-      <c r="F35" s="4">
-        <v>0</v>
-      </c>
-      <c r="G35" s="5">
-        <v>1</v>
-      </c>
-      <c r="H35" s="5">
+      <c r="F35" s="3">
+        <v>0</v>
+      </c>
+      <c r="G35" s="4">
+        <v>1</v>
+      </c>
+      <c r="H35" s="4">
         <v>10.199999999999999</v>
       </c>
-      <c r="I35" s="35">
-        <f ca="1">(H35-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
+      <c r="I35" s="17">
+        <f t="shared" ca="1" si="0"/>
         <v>0.57594936708860767</v>
       </c>
-      <c r="J35" s="36">
+      <c r="J35" s="18">
         <f ca="1">1.2*C35 + 1.2*D35 + 0.5*E35 + F35 + G35 - I35 - 0.1*K35</f>
         <v>0.32405063291139236</v>
       </c>
       <c r="K35">
         <v>1</v>
       </c>
-      <c r="L35" s="22">
+      <c r="L35" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B36" s="10" t="s">
         <v>30</v>
-      </c>
-      <c r="B36" s="22" t="s">
-        <v>31</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -2701,27 +2312,27 @@
       <c r="H36">
         <v>10.9</v>
       </c>
-      <c r="I36" s="35">
-        <f ca="1">(H36-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
+      <c r="I36" s="17">
+        <f t="shared" ca="1" si="0"/>
         <v>0.62025316455696211</v>
       </c>
-      <c r="J36" s="36">
-        <f t="shared" ref="J36:J47" ca="1" si="1">1.2*C36 + 1.2*D36 + 0.5*E36 + F36 + G36 - I36 - 0.15*K36</f>
+      <c r="J36" s="18">
+        <f t="shared" ref="J36:J47" ca="1" si="2">1.2*C36 + 1.2*D36 + 0.5*E36 + F36 + G36 - I36 - 0.15*K36</f>
         <v>7.97468354430379E-2</v>
       </c>
       <c r="K36">
         <v>2</v>
       </c>
-      <c r="L36" s="22">
+      <c r="L36" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37" s="10" t="s">
         <v>45</v>
-      </c>
-      <c r="B37" s="22" t="s">
-        <v>46</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -2741,27 +2352,27 @@
       <c r="H37">
         <v>9.1</v>
       </c>
-      <c r="I37" s="35">
-        <f ca="1">(H37-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
+      <c r="I37" s="17">
+        <f t="shared" ca="1" si="0"/>
         <v>0.50632911392405067</v>
       </c>
-      <c r="J37" s="36">
-        <f t="shared" ca="1" si="1"/>
+      <c r="J37" s="18">
+        <f t="shared" ca="1" si="2"/>
         <v>4.3670886075949378E-2</v>
       </c>
       <c r="K37">
         <v>3</v>
       </c>
-      <c r="L37" s="22">
+      <c r="L37" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38" s="10" t="s">
         <v>47</v>
-      </c>
-      <c r="B38" s="22" t="s">
-        <v>48</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -2781,27 +2392,27 @@
       <c r="H38">
         <v>12</v>
       </c>
-      <c r="I38" s="35">
-        <f ca="1">(H38-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
+      <c r="I38" s="17">
+        <f t="shared" ca="1" si="0"/>
         <v>0.68987341772151911</v>
       </c>
-      <c r="J38" s="36">
-        <f t="shared" ca="1" si="1"/>
+      <c r="J38" s="18">
+        <f t="shared" ca="1" si="2"/>
         <v>1.01265822784809E-2</v>
       </c>
       <c r="K38">
         <v>2</v>
       </c>
-      <c r="L38" s="22">
+      <c r="L38" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B39" s="10" t="s">
         <v>16</v>
-      </c>
-      <c r="B39" s="22" t="s">
-        <v>17</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -2821,27 +2432,27 @@
       <c r="H39">
         <v>4.5</v>
       </c>
-      <c r="I39" s="35">
-        <f ca="1">(H39-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
+      <c r="I39" s="17">
+        <f t="shared" ca="1" si="0"/>
         <v>0.21518987341772153</v>
       </c>
-      <c r="J39" s="36">
-        <f t="shared" ca="1" si="1"/>
+      <c r="J39" s="18">
+        <f t="shared" ca="1" si="2"/>
         <v>-1.5189873417721544E-2</v>
       </c>
       <c r="K39">
         <v>2</v>
       </c>
-      <c r="L39" s="22">
+      <c r="L39" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B40" s="10" t="s">
         <v>49</v>
-      </c>
-      <c r="B40" s="22" t="s">
-        <v>50</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -2861,27 +2472,27 @@
       <c r="H40">
         <v>6.5</v>
       </c>
-      <c r="I40" s="35">
-        <f ca="1">(H40-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
+      <c r="I40" s="17">
+        <f t="shared" ca="1" si="0"/>
         <v>0.34177215189873422</v>
       </c>
-      <c r="J40" s="36">
-        <f t="shared" ca="1" si="1"/>
+      <c r="J40" s="18">
+        <f t="shared" ca="1" si="2"/>
         <v>-0.14177215189873421</v>
       </c>
       <c r="K40">
         <v>2</v>
       </c>
-      <c r="L40" s="22">
+      <c r="L40" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B41" s="10" t="s">
         <v>67</v>
-      </c>
-      <c r="B41" s="22" t="s">
-        <v>68</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -2901,27 +2512,27 @@
       <c r="H41">
         <v>4.3</v>
       </c>
-      <c r="I41" s="35">
-        <f ca="1">(H41-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
+      <c r="I41" s="17">
+        <f t="shared" ca="1" si="0"/>
         <v>0.20253164556962025</v>
       </c>
-      <c r="J41" s="36">
-        <f t="shared" ca="1" si="1"/>
+      <c r="J41" s="18">
+        <f t="shared" ca="1" si="2"/>
         <v>-0.15253164556962018</v>
       </c>
       <c r="K41">
         <v>3</v>
       </c>
-      <c r="L41" s="22">
+      <c r="L41" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B42" s="22" t="s">
-        <v>38</v>
+        <v>100</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>37</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -2941,27 +2552,27 @@
       <c r="H42">
         <v>12.3</v>
       </c>
-      <c r="I42" s="35">
-        <f ca="1">(H42-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
+      <c r="I42" s="17">
+        <f t="shared" ca="1" si="0"/>
         <v>0.708860759493671</v>
       </c>
-      <c r="J42" s="36">
-        <f t="shared" ca="1" si="1"/>
+      <c r="J42" s="18">
+        <f t="shared" ca="1" si="2"/>
         <v>-0.15886075949367096</v>
       </c>
       <c r="K42">
         <v>3</v>
       </c>
-      <c r="L42" s="22">
+      <c r="L42" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43" s="10" t="s">
         <v>41</v>
-      </c>
-      <c r="B43" s="22" t="s">
-        <v>42</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -2981,27 +2592,27 @@
       <c r="H43">
         <v>7.1</v>
       </c>
-      <c r="I43" s="35">
-        <f ca="1">(H43-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
+      <c r="I43" s="17">
+        <f t="shared" ca="1" si="0"/>
         <v>0.379746835443038</v>
       </c>
-      <c r="J43" s="36">
-        <f t="shared" ca="1" si="1"/>
+      <c r="J43" s="18">
+        <f t="shared" ca="1" si="2"/>
         <v>-0.17974683544303799</v>
       </c>
       <c r="K43">
         <v>2</v>
       </c>
-      <c r="L43" s="22">
+      <c r="L43" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B44" s="10" t="s">
         <v>36</v>
-      </c>
-      <c r="B44" s="22" t="s">
-        <v>37</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -3021,18 +2632,18 @@
       <c r="H44">
         <v>9.8000000000000007</v>
       </c>
-      <c r="I44" s="35">
-        <f ca="1">(H44-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
+      <c r="I44" s="17">
+        <f t="shared" ca="1" si="0"/>
         <v>0.55063291139240522</v>
       </c>
-      <c r="J44" s="36">
-        <f t="shared" ca="1" si="1"/>
+      <c r="J44" s="18">
+        <f t="shared" ca="1" si="2"/>
         <v>-0.35063291139240521</v>
       </c>
       <c r="K44">
         <v>2</v>
       </c>
-      <c r="L44" s="22">
+      <c r="L44" s="10">
         <v>1</v>
       </c>
     </row>
@@ -3040,7 +2651,7 @@
       <c r="A45" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="22" t="s">
+      <c r="B45" s="10" t="s">
         <v>14</v>
       </c>
       <c r="C45">
@@ -3061,27 +2672,27 @@
       <c r="H45">
         <v>8.9</v>
       </c>
-      <c r="I45" s="35">
-        <f ca="1">(H45-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
+      <c r="I45" s="17">
+        <f t="shared" ca="1" si="0"/>
         <v>0.49367088607594944</v>
       </c>
-      <c r="J45" s="36">
-        <f t="shared" ca="1" si="1"/>
+      <c r="J45" s="18">
+        <f t="shared" ca="1" si="2"/>
         <v>-0.4436708860759494</v>
       </c>
       <c r="K45">
         <v>3</v>
       </c>
-      <c r="L45" s="22">
+      <c r="L45" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B46" s="10" t="s">
         <v>28</v>
-      </c>
-      <c r="B46" s="22" t="s">
-        <v>29</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -3101,58 +2712,58 @@
       <c r="H46">
         <v>16.899999999999999</v>
       </c>
-      <c r="I46" s="35">
-        <f ca="1">(H46-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
-        <v>1</v>
-      </c>
-      <c r="J46" s="36">
-        <f t="shared" ca="1" si="1"/>
+      <c r="I46" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J46" s="18">
+        <f t="shared" ca="1" si="2"/>
         <v>-0.44999999999999996</v>
       </c>
       <c r="K46">
         <v>3</v>
       </c>
-      <c r="L46" s="22">
+      <c r="L46" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="38" t="s">
+      <c r="A47" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B47" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B47" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="C47" s="23">
-        <v>0</v>
-      </c>
-      <c r="D47" s="23">
-        <v>0</v>
-      </c>
-      <c r="E47" s="23">
-        <v>1</v>
-      </c>
-      <c r="F47" s="23">
-        <v>0</v>
-      </c>
-      <c r="G47" s="23">
-        <v>0</v>
-      </c>
-      <c r="H47" s="23">
+      <c r="C47" s="11">
+        <v>0</v>
+      </c>
+      <c r="D47" s="11">
+        <v>0</v>
+      </c>
+      <c r="E47" s="11">
+        <v>1</v>
+      </c>
+      <c r="F47" s="11">
+        <v>0</v>
+      </c>
+      <c r="G47" s="11">
+        <v>0</v>
+      </c>
+      <c r="H47" s="11">
         <v>11.8</v>
       </c>
-      <c r="I47" s="37">
-        <f ca="1">(H47-MIN(J:J))/(MAX(J:J)-MIN(J:J))</f>
+      <c r="I47" s="19">
+        <f t="shared" ca="1" si="0"/>
         <v>0.67721518987341789</v>
       </c>
-      <c r="J47" s="36">
-        <f t="shared" ca="1" si="1"/>
+      <c r="J47" s="18">
+        <f t="shared" ca="1" si="2"/>
         <v>-0.47721518987341788</v>
       </c>
-      <c r="K47" s="23">
+      <c r="K47" s="11">
         <v>2</v>
       </c>
-      <c r="L47" s="24">
+      <c r="L47" s="12">
         <v>1</v>
       </c>
     </row>
@@ -3166,251 +2777,251 @@
     </row>
     <row r="50" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C50"/>
-      <c r="H50" s="4"/>
-      <c r="I50" s="5"/>
-      <c r="J50" s="5"/>
+      <c r="H50" s="3"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
     </row>
     <row r="51" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C51"/>
-      <c r="H51" s="4"/>
-      <c r="I51" s="5"/>
-      <c r="J51" s="5"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="4"/>
+      <c r="J51" s="4"/>
     </row>
     <row r="52" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C52"/>
-      <c r="H52" s="4"/>
-      <c r="I52" s="5"/>
-      <c r="J52" s="5"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="4"/>
     </row>
     <row r="53" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C53"/>
-      <c r="H53" s="4"/>
-      <c r="I53" s="5"/>
-      <c r="J53" s="5"/>
+      <c r="H53" s="3"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="4"/>
     </row>
     <row r="54" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="55" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C55" s="7"/>
+      <c r="C55" s="6"/>
       <c r="D55" s="2"/>
     </row>
     <row r="56" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C56" s="15"/>
-      <c r="D56" s="15"/>
-      <c r="E56" s="10"/>
-      <c r="F56" s="10"/>
-      <c r="G56" s="10"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="8"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="7"/>
     </row>
     <row r="57" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C57" s="15"/>
-      <c r="D57" s="15"/>
-      <c r="E57" s="10"/>
-      <c r="F57" s="10"/>
-      <c r="G57" s="10"/>
+      <c r="C57" s="8"/>
+      <c r="D57" s="8"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="7"/>
     </row>
     <row r="58" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C58" s="15"/>
-      <c r="D58" s="15"/>
-      <c r="E58" s="10"/>
-      <c r="F58" s="10"/>
-      <c r="G58" s="10"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
+      <c r="E58" s="7"/>
+      <c r="F58" s="7"/>
+      <c r="G58" s="7"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C59" s="15"/>
-      <c r="D59" s="15"/>
-      <c r="E59" s="10"/>
-      <c r="F59" s="10"/>
-      <c r="G59" s="10"/>
+      <c r="C59" s="8"/>
+      <c r="D59" s="8"/>
+      <c r="E59" s="7"/>
+      <c r="F59" s="7"/>
+      <c r="G59" s="7"/>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C60" s="15"/>
-      <c r="D60" s="15"/>
-      <c r="E60" s="10"/>
-      <c r="F60" s="10"/>
-      <c r="G60" s="10"/>
+      <c r="C60" s="8"/>
+      <c r="D60" s="8"/>
+      <c r="E60" s="7"/>
+      <c r="F60" s="7"/>
+      <c r="G60" s="7"/>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C61" s="15"/>
-      <c r="D61" s="15"/>
-      <c r="E61" s="10"/>
-      <c r="F61" s="10"/>
-      <c r="G61" s="10"/>
+      <c r="C61" s="8"/>
+      <c r="D61" s="8"/>
+      <c r="E61" s="7"/>
+      <c r="F61" s="7"/>
+      <c r="G61" s="7"/>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C62" s="15"/>
-      <c r="D62" s="15"/>
-      <c r="E62" s="10"/>
-      <c r="F62" s="10"/>
-      <c r="G62" s="10"/>
+      <c r="C62" s="8"/>
+      <c r="D62" s="8"/>
+      <c r="E62" s="7"/>
+      <c r="F62" s="7"/>
+      <c r="G62" s="7"/>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C63" s="15"/>
-      <c r="D63" s="15"/>
-      <c r="E63" s="10"/>
-      <c r="F63" s="10"/>
-      <c r="G63" s="10"/>
+      <c r="C63" s="8"/>
+      <c r="D63" s="8"/>
+      <c r="E63" s="7"/>
+      <c r="F63" s="7"/>
+      <c r="G63" s="7"/>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C64" s="15"/>
-      <c r="D64" s="15"/>
-      <c r="E64" s="10"/>
-      <c r="F64" s="10"/>
-      <c r="G64" s="10"/>
+      <c r="C64" s="8"/>
+      <c r="D64" s="8"/>
+      <c r="E64" s="7"/>
+      <c r="F64" s="7"/>
+      <c r="G64" s="7"/>
     </row>
     <row r="65" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C65" s="15"/>
-      <c r="D65" s="15"/>
-      <c r="E65" s="10"/>
-      <c r="F65" s="10"/>
-      <c r="G65" s="10"/>
+      <c r="C65" s="8"/>
+      <c r="D65" s="8"/>
+      <c r="E65" s="7"/>
+      <c r="F65" s="7"/>
+      <c r="G65" s="7"/>
     </row>
     <row r="66" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C66" s="15"/>
-      <c r="D66" s="15"/>
-      <c r="E66" s="10"/>
-      <c r="F66" s="10"/>
-      <c r="G66" s="10"/>
+      <c r="C66" s="8"/>
+      <c r="D66" s="8"/>
+      <c r="E66" s="7"/>
+      <c r="F66" s="7"/>
+      <c r="G66" s="7"/>
     </row>
     <row r="67" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C67" s="15"/>
-      <c r="D67" s="15"/>
-      <c r="E67" s="10"/>
-      <c r="F67" s="10"/>
-      <c r="G67" s="10"/>
+      <c r="C67" s="8"/>
+      <c r="D67" s="8"/>
+      <c r="E67" s="7"/>
+      <c r="F67" s="7"/>
+      <c r="G67" s="7"/>
     </row>
     <row r="68" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C68" s="15"/>
-      <c r="D68" s="15"/>
-      <c r="E68" s="10"/>
-      <c r="F68" s="10"/>
-      <c r="G68" s="10"/>
+      <c r="C68" s="8"/>
+      <c r="D68" s="8"/>
+      <c r="E68" s="7"/>
+      <c r="F68" s="7"/>
+      <c r="G68" s="7"/>
     </row>
     <row r="69" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C69" s="15"/>
-      <c r="D69" s="15"/>
-      <c r="E69" s="10"/>
-      <c r="F69" s="10"/>
-      <c r="G69" s="10"/>
+      <c r="C69" s="8"/>
+      <c r="D69" s="8"/>
+      <c r="E69" s="7"/>
+      <c r="F69" s="7"/>
+      <c r="G69" s="7"/>
     </row>
     <row r="70" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C70" s="15"/>
-      <c r="D70" s="15"/>
-      <c r="E70" s="10"/>
-      <c r="F70" s="10"/>
-      <c r="G70" s="10"/>
-      <c r="I70" s="16"/>
+      <c r="C70" s="8"/>
+      <c r="D70" s="8"/>
+      <c r="E70" s="7"/>
+      <c r="F70" s="7"/>
+      <c r="G70" s="7"/>
+      <c r="I70" s="9"/>
     </row>
     <row r="71" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C71" s="15"/>
-      <c r="D71" s="15"/>
-      <c r="E71" s="10"/>
-      <c r="F71" s="10"/>
-      <c r="G71" s="10"/>
-      <c r="I71" s="16"/>
+      <c r="C71" s="8"/>
+      <c r="D71" s="8"/>
+      <c r="E71" s="7"/>
+      <c r="F71" s="7"/>
+      <c r="G71" s="7"/>
+      <c r="I71" s="9"/>
     </row>
     <row r="72" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C72" s="15"/>
-      <c r="D72" s="15"/>
-      <c r="E72" s="10"/>
-      <c r="F72" s="10"/>
-      <c r="G72" s="10"/>
-      <c r="I72" s="16"/>
+      <c r="C72" s="8"/>
+      <c r="D72" s="8"/>
+      <c r="E72" s="7"/>
+      <c r="F72" s="7"/>
+      <c r="G72" s="7"/>
+      <c r="I72" s="9"/>
     </row>
     <row r="73" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C73" s="15"/>
-      <c r="D73" s="15"/>
-      <c r="E73" s="10"/>
-      <c r="F73" s="10"/>
-      <c r="G73" s="10"/>
-      <c r="I73" s="16"/>
+      <c r="C73" s="8"/>
+      <c r="D73" s="8"/>
+      <c r="E73" s="7"/>
+      <c r="F73" s="7"/>
+      <c r="G73" s="7"/>
+      <c r="I73" s="9"/>
     </row>
     <row r="74" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C74" s="15"/>
-      <c r="D74" s="15"/>
-      <c r="E74" s="10"/>
-      <c r="F74" s="10"/>
-      <c r="G74" s="10"/>
-      <c r="I74" s="16"/>
+      <c r="C74" s="8"/>
+      <c r="D74" s="8"/>
+      <c r="E74" s="7"/>
+      <c r="F74" s="7"/>
+      <c r="G74" s="7"/>
+      <c r="I74" s="9"/>
     </row>
     <row r="75" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C75" s="15"/>
-      <c r="D75" s="15"/>
-      <c r="E75" s="10"/>
-      <c r="F75" s="10"/>
-      <c r="G75" s="10"/>
-      <c r="I75" s="16"/>
+      <c r="C75" s="8"/>
+      <c r="D75" s="8"/>
+      <c r="E75" s="7"/>
+      <c r="F75" s="7"/>
+      <c r="G75" s="7"/>
+      <c r="I75" s="9"/>
     </row>
     <row r="76" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C76" s="15"/>
-      <c r="D76" s="15"/>
-      <c r="E76" s="10"/>
-      <c r="F76" s="10"/>
-      <c r="G76" s="10"/>
-      <c r="I76" s="16"/>
+      <c r="C76" s="8"/>
+      <c r="D76" s="8"/>
+      <c r="E76" s="7"/>
+      <c r="F76" s="7"/>
+      <c r="G76" s="7"/>
+      <c r="I76" s="9"/>
     </row>
     <row r="77" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C77" s="10"/>
-      <c r="D77" s="10"/>
-      <c r="E77" s="10"/>
-      <c r="F77" s="10"/>
-      <c r="G77" s="10"/>
-      <c r="I77" s="16"/>
+      <c r="C77" s="7"/>
+      <c r="D77" s="7"/>
+      <c r="E77" s="7"/>
+      <c r="F77" s="7"/>
+      <c r="G77" s="7"/>
+      <c r="I77" s="9"/>
     </row>
     <row r="78" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C78" s="10"/>
-      <c r="D78" s="10"/>
-      <c r="E78" s="10"/>
-      <c r="F78" s="10"/>
-      <c r="G78" s="10"/>
-      <c r="I78" s="16"/>
+      <c r="C78" s="7"/>
+      <c r="D78" s="7"/>
+      <c r="E78" s="7"/>
+      <c r="F78" s="7"/>
+      <c r="G78" s="7"/>
+      <c r="I78" s="9"/>
     </row>
     <row r="79" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C79" s="10"/>
-      <c r="D79" s="10"/>
-      <c r="E79" s="10"/>
-      <c r="F79" s="10"/>
-      <c r="G79" s="10"/>
+      <c r="C79" s="7"/>
+      <c r="D79" s="7"/>
+      <c r="E79" s="7"/>
+      <c r="F79" s="7"/>
+      <c r="G79" s="7"/>
     </row>
     <row r="80" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C80" s="10"/>
-      <c r="D80" s="10"/>
-      <c r="E80" s="10"/>
-      <c r="F80" s="10"/>
-      <c r="G80" s="10"/>
+      <c r="C80" s="7"/>
+      <c r="D80" s="7"/>
+      <c r="E80" s="7"/>
+      <c r="F80" s="7"/>
+      <c r="G80" s="7"/>
     </row>
     <row r="81" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C81" s="10"/>
-      <c r="D81" s="10"/>
-      <c r="E81" s="10"/>
-      <c r="F81" s="10"/>
-      <c r="G81" s="10"/>
+      <c r="C81" s="7"/>
+      <c r="D81" s="7"/>
+      <c r="E81" s="7"/>
+      <c r="F81" s="7"/>
+      <c r="G81" s="7"/>
     </row>
     <row r="82" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C82" s="10"/>
-      <c r="D82" s="10"/>
-      <c r="E82" s="10"/>
-      <c r="F82" s="10"/>
-      <c r="G82" s="10"/>
+      <c r="C82" s="7"/>
+      <c r="D82" s="7"/>
+      <c r="E82" s="7"/>
+      <c r="F82" s="7"/>
+      <c r="G82" s="7"/>
     </row>
     <row r="83" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C83" s="10"/>
-      <c r="D83" s="10"/>
-      <c r="E83" s="10"/>
-      <c r="F83" s="10"/>
-      <c r="G83" s="10"/>
+      <c r="C83" s="7"/>
+      <c r="D83" s="7"/>
+      <c r="E83" s="7"/>
+      <c r="F83" s="7"/>
+      <c r="G83" s="7"/>
     </row>
     <row r="84" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C84" s="10"/>
-      <c r="D84" s="10"/>
-      <c r="E84" s="10"/>
-      <c r="F84" s="10"/>
-      <c r="G84" s="10"/>
+      <c r="C84" s="7"/>
+      <c r="D84" s="7"/>
+      <c r="E84" s="7"/>
+      <c r="F84" s="7"/>
+      <c r="G84" s="7"/>
     </row>
     <row r="85" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C85" s="10"/>
-      <c r="D85" s="10"/>
-      <c r="E85" s="10"/>
-      <c r="F85" s="10"/>
-      <c r="G85" s="10"/>
+      <c r="C85" s="7"/>
+      <c r="D85" s="7"/>
+      <c r="E85" s="7"/>
+      <c r="F85" s="7"/>
+      <c r="G85" s="7"/>
     </row>
     <row r="86" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C86"/>
@@ -3498,649 +3109,4 @@
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DB2EAD1-E4AE-4551-B257-795479122738}">
-  <dimension ref="B3:J52"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScale="48" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="87.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="54.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B3" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="H3" s="4"/>
-    </row>
-    <row r="4" spans="2:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="B4" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="F4" s="30" t="s">
-        <v>102</v>
-      </c>
-      <c r="G4" s="30" t="s">
-        <v>186</v>
-      </c>
-      <c r="H4" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="30" t="s">
-        <v>187</v>
-      </c>
-      <c r="J4" s="30" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B5" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B6" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B7" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B8" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B9" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B10" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B11" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B12" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D12" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="E12" s="25" t="s">
-        <v>129</v>
-      </c>
-      <c r="F12" s="25" t="s">
-        <v>130</v>
-      </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B15" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="G15" s="3">
-        <v>0</v>
-      </c>
-      <c r="H15" s="28"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B16" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="G16" s="3"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B17" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="G17" s="3">
-        <v>0</v>
-      </c>
-      <c r="H17" s="3">
-        <v>1</v>
-      </c>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B18" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="G18" s="3">
-        <v>0</v>
-      </c>
-      <c r="H18" s="3">
-        <v>1</v>
-      </c>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B19" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B20" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B21" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3">
-        <v>1</v>
-      </c>
-      <c r="J21" s="3"/>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B22" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="G22" s="3">
-        <v>1</v>
-      </c>
-      <c r="H22" s="3">
-        <v>1</v>
-      </c>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B23" s="13" t="s">
-        <v>162</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="D23" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="G23" s="26"/>
-      <c r="H23" s="29"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="26"/>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="H24" s="4"/>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="H25" s="4"/>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="H26" s="4"/>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="H27" s="4"/>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="H28" s="4"/>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="H29" s="4"/>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B30" s="6"/>
-      <c r="H30" s="4"/>
-    </row>
-    <row r="31" spans="2:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="B31" s="17" t="s">
-        <v>165</v>
-      </c>
-      <c r="H31" s="4"/>
-    </row>
-    <row r="32" spans="2:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="B32" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="H32" s="4"/>
-    </row>
-    <row r="33" spans="2:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="B33" s="19" t="s">
-        <v>167</v>
-      </c>
-      <c r="H33" s="4"/>
-    </row>
-    <row r="34" spans="2:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="B34" s="19" t="s">
-        <v>168</v>
-      </c>
-      <c r="H34" s="4"/>
-    </row>
-    <row r="35" spans="2:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="B35" s="19" t="s">
-        <v>169</v>
-      </c>
-      <c r="H35" s="4"/>
-    </row>
-    <row r="36" spans="2:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="B36" s="19" t="s">
-        <v>170</v>
-      </c>
-      <c r="H36" s="4"/>
-    </row>
-    <row r="37" spans="2:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="B37" s="19" t="s">
-        <v>171</v>
-      </c>
-      <c r="H37" s="4"/>
-    </row>
-    <row r="38" spans="2:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="B38" s="19" t="s">
-        <v>172</v>
-      </c>
-      <c r="H38" s="4"/>
-    </row>
-    <row r="39" spans="2:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="B39" s="19" t="s">
-        <v>173</v>
-      </c>
-      <c r="H39" s="4"/>
-    </row>
-    <row r="40" spans="2:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="B40" s="19" t="s">
-        <v>174</v>
-      </c>
-      <c r="H40" s="4"/>
-    </row>
-    <row r="41" spans="2:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="B41" s="20" t="s">
-        <v>175</v>
-      </c>
-      <c r="H41" s="4"/>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B42" s="6"/>
-      <c r="H42" s="4"/>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B43" s="6"/>
-      <c r="H43" s="4"/>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B44" s="6"/>
-      <c r="H44" s="4"/>
-    </row>
-    <row r="45" spans="2:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="B45" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="H45" s="4"/>
-    </row>
-    <row r="46" spans="2:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="B46" s="21" t="s">
-        <v>177</v>
-      </c>
-      <c r="H46" s="4"/>
-    </row>
-    <row r="47" spans="2:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="B47" s="19" t="s">
-        <v>178</v>
-      </c>
-      <c r="H47" s="4"/>
-    </row>
-    <row r="48" spans="2:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="B48" s="19" t="s">
-        <v>179</v>
-      </c>
-      <c r="H48" s="4"/>
-    </row>
-    <row r="49" spans="2:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="B49" s="19" t="s">
-        <v>180</v>
-      </c>
-      <c r="H49" s="4"/>
-    </row>
-    <row r="50" spans="2:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="B50" s="19" t="s">
-        <v>181</v>
-      </c>
-      <c r="H50" s="4"/>
-    </row>
-    <row r="51" spans="2:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="B51" s="19" t="s">
-        <v>182</v>
-      </c>
-      <c r="H51" s="4"/>
-    </row>
-    <row r="52" spans="2:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="B52" s="20" t="s">
-        <v>183</v>
-      </c>
-      <c r="H52" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>